<commit_message>
Revising upload template of users
</commit_message>
<xml_diff>
--- a/uploads/UPLOAD-TEMPLATE/USERS-UPLOAD-TEMPLATE.xlsx
+++ b/uploads/UPLOAD-TEMPLATE/USERS-UPLOAD-TEMPLATE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\node proj\rest-api-nestjs\uploads\UPLOAD-TEMPLATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238CBBC8-2A54-4306-BAAB-AF1879293B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E06E51-27BE-4AC9-8809-88F0F3F5F6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2592" yWindow="1404" windowWidth="17280" windowHeight="9420" xr2:uid="{8DE630E0-0B89-4DDE-A92E-DF514EA9A919}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8DE630E0-0B89-4DDE-A92E-DF514EA9A919}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,35 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>* First Name</t>
-  </si>
-  <si>
-    <t>* Last Name</t>
-  </si>
-  <si>
-    <t>* Email</t>
-  </si>
-  <si>
-    <t>* Employee No.</t>
-  </si>
-  <si>
-    <t>* Password</t>
-  </si>
-  <si>
-    <t>* Username</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Middle Name</t>
   </si>
   <si>
-    <t>* Access Keys</t>
-  </si>
-  <si>
-    <t>* Role</t>
-  </si>
-  <si>
     <t>User Reset</t>
   </si>
   <si>
@@ -76,13 +52,46 @@
   </si>
   <si>
     <t>ADMIN</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Employee No.</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Access Keys</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Location(s)</t>
+  </si>
+  <si>
+    <t>METRO MANILA, CENTRAL LUZON</t>
+  </si>
+  <si>
+    <t>* delete this line and above sample data on actual uploading</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,8 +122,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +141,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -141,11 +164,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -461,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAE589B1-C7BA-44D4-9E29-919A5892AA9B}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,68 +503,79 @@
     <col min="7" max="7" width="14.77734375" customWidth="1"/>
     <col min="8" max="8" width="16.109375" customWidth="1"/>
     <col min="9" max="9" width="15.21875" customWidth="1"/>
-    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>10</v>
       </c>
       <c r="B2">
         <v>12345678</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>